<commit_message>
SON24 new content: Charts and tables: IN13 Attainment at age 16: Review mark-ups
</commit_message>
<xml_diff>
--- a/son/content/intermediate_outcomes/compulsory_school_age_(5_to_16_years)/attainment_at_age_16/2.0/IN13-2.0-attainment-at-age-16--by-year-and-disadvantage--table-format.xlsx
+++ b/son/content/intermediate_outcomes/compulsory_school_age_(5_to_16_years)/attainment_at_age_16/2.0/IN13-2.0-attainment-at-age-16--by-year-and-disadvantage--table-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\intermediate_outcomes\compulsory_school_age_(5_to_16_years)\attainment_at_age_16\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF131B72-51AC-4615-B8DB-B3EFA8C6CE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BEE6B8-5C97-4ED5-A0FB-49DD6C757643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{71FCE1DA-95D3-4354-B9E6-4AD770BF0FBD}"/>
   </bookViews>
@@ -21,13 +21,13 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4368" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4369" uniqueCount="105">
   <si>
     <t>ind_code</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Not known to be disadvantaged (%)</t>
+  </si>
+  <si>
+    <t>Total (%)</t>
   </si>
 </sst>
 </file>
@@ -6872,8 +6875,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FD2FE0A8-D145-4509-890E-905E89AB7BF8}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="School year">
-  <location ref="A5:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FD2FE0A8-D145-4509-890E-905E89AB7BF8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="School year">
+  <location ref="A5:D11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -6913,7 +6916,7 @@
         <item h="1" x="5"/>
         <item n="Not known to be disadvantaged (%)" x="3"/>
         <item h="1" x="1"/>
-        <item h="1" x="4"/>
+        <item n="Total (%)" x="4"/>
         <item h="1" x="6"/>
         <item t="default"/>
       </items>
@@ -6971,12 +6974,15 @@
   <colFields count="1">
     <field x="6"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="3">
     <i>
       <x/>
     </i>
     <i>
       <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
   </colItems>
   <pageFields count="3">
@@ -7327,10 +7333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3613E48C-BCEF-4328-A4DF-FCC0EE7CA4E7}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7338,14 +7344,14 @@
     <col min="1" max="1" width="12.765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.4609375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.07421875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.07421875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.84375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7353,7 +7359,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -7361,7 +7367,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -7369,7 +7375,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -7377,7 +7383,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -7387,8 +7393,11 @@
       <c r="C6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>97</v>
       </c>
@@ -7398,8 +7407,11 @@
       <c r="C7" s="3">
         <v>52.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D7" s="3">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>98</v>
       </c>
@@ -7409,8 +7421,11 @@
       <c r="C8" s="3">
         <v>57.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D8" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>99</v>
       </c>
@@ -7420,8 +7435,11 @@
       <c r="C9" s="3">
         <v>59.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D9" s="3">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>100</v>
       </c>
@@ -7431,8 +7449,11 @@
       <c r="C10" s="3">
         <v>56.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D10" s="3">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>101</v>
       </c>
@@ -7441,6 +7462,9 @@
       </c>
       <c r="C11" s="3">
         <v>50.1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>43.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>